<commit_message>
Menambah atribut -t whole
</commit_message>
<xml_diff>
--- a/playground/read_table/temp.xlsx
+++ b/playground/read_table/temp.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,10 +480,20 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Max Port</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Ready Port</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>First Updated</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Last Updated</t>
         </is>
@@ -522,8 +532,12 @@
           <t>ODP-MAT-FBM/080</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" s="2" t="n">
+      <c r="I2" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" s="2" t="n">
         <v>45475</v>
       </c>
     </row>
@@ -560,8 +574,12 @@
           <t>ODP-MAT-FF/13</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" s="2" t="n">
+      <c r="I3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" s="2" t="n">
         <v>45475</v>
       </c>
     </row>
@@ -592,7 +610,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>22990465</t>
+          <t>22990459</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -600,13 +618,17 @@
           <t>ODP-MAT-FBW/029</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>16</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
         <is>
           <t>2024-02-11 14:50:16</t>
         </is>
       </c>
-      <c r="J4" s="2" t="n">
-        <v>45333.61848379629</v>
+      <c r="L4" s="2" t="n">
+        <v>45333.70420138889</v>
       </c>
     </row>
     <row r="5">
@@ -640,8 +662,12 @@
           <t>ODP-MAT-FS/049</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>8</v>
+      </c>
       <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -674,8 +700,12 @@
           <t>ODP-MAT-FW/033</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>16</v>
+      </c>
       <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -704,8 +734,12 @@
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>8</v>
+      </c>
       <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -734,8 +768,12 @@
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>16</v>
+      </c>
       <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -764,8 +802,12 @@
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>8</v>
+      </c>
       <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>